<commit_message>
add neural decision tree
</commit_message>
<xml_diff>
--- a/nn_clustering.xlsx
+++ b/nn_clustering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzhao\PycharmProjects\fedod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4F0729-A0A6-4C27-9559-55A0F11D6748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98436D7-0ACB-4324-BB49-F56E830FEAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25507" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{F5986BF2-57FA-0542-91DB-C4C511282E6F}"/>
+    <workbookView xWindow="26773" yWindow="1120" windowWidth="19200" windowHeight="12560" xr2:uid="{F5986BF2-57FA-0542-91DB-C4C511282E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="annthyroid" sheetId="1" r:id="rId1"/>
@@ -484,14 +484,16 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -546,6 +548,9 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
+      <c r="E4" s="1">
+        <v>0.72915092926810698</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
@@ -557,6 +562,9 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
+      <c r="E5" s="1">
+        <v>0.66474250141477798</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
@@ -568,6 +576,9 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
+      <c r="E6" s="1">
+        <v>0.64040108543285801</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
@@ -579,6 +590,9 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
+      <c r="E7" s="1">
+        <v>0.65626784031383101</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
@@ -590,6 +604,9 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
+      <c r="E8" s="1">
+        <v>0.65978107304381195</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
@@ -601,6 +618,9 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
+      <c r="E9" s="1">
+        <v>0.685273675720388</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
@@ -612,6 +632,9 @@
       <c r="D10" s="1">
         <v>9</v>
       </c>
+      <c r="E10" s="1">
+        <v>0.68448145683087902</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
@@ -623,6 +646,9 @@
       <c r="D11" s="1">
         <v>10</v>
       </c>
+      <c r="E11" s="1">
+        <v>0.63545825106632103</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
@@ -637,7 +663,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" ref="E12" si="1">AVERAGE(E2:E11)</f>
-        <v>0.63350176217280008</v>
+        <v>0.66225603374365738</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>